<commit_message>
Some more bugs on the "magazin" page
</commit_message>
<xml_diff>
--- a/Собаседник-bug report.xlsx
+++ b/Собаседник-bug report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="147">
   <si>
     <t xml:space="preserve">Шаблон для тестирования сайта Собаседник.</t>
   </si>
@@ -486,6 +486,148 @@
   </si>
   <si>
     <t xml:space="preserve">SOB_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 на странице магазина добавить любой товар в любом количестве в корзину по кнопке “купить”, перейти в корзину</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Нажать кнопку “оформить заказ”
+3 На открывшейся странице ввести в поля валидные данные, внизу нажать на кнопку “далее”
+4 Выбрать “наличными курьеру”, нажать “далее”
+5 Выбрать “стандартная”, нажать “далее”
+6 Прокрутить заказ вниз, поставить галочку на “Правило и право возврата”, нажать “подтвердить заказ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Происходит возврат на страницу ввода личных данных и наверху страницы табличка “Внимание”, а под ней ошибка “Could not instantiate mail function.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Происходит завершение процесса совершения заказа, появляется сообщение об успешном создании заказа с информацией.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOB_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 на странице магазина обратить внимание на надпись “нет в наличии” под фотографией каждого товара
+2 добавить любой товар в любом количестве в корзину по кнопке “купить”, перейти в корзину</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 нажать кнопку “оформить заказ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Происходит переход на страничку ввода личных данных и далее вплоть до завершения создания заказа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Невозможно добавить в корзину товар, которого нет в наличии, невозможно из корзины перейти к оформлению, если товара нет в наличии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOB_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 на странице магазина обратить внимание на цену на карточке товара “Перекус для собачки”: 117.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 перейти на карточку данного товара любым способом (клик на изображение, клик на название товара, клик на кнопку “купить” или “подробнее”)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена меняется и, несмотря на то что мясо доступно в двух цветах, “red” и “blue”, цены в 117.30 нигде нет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В карточке товара у одного из вариантов покупки есть цена соответствующая цене на главной странице магазина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOB_21</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> на странице магазина перейти на карточку товара “Выпуск подкаста” </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">любым способом (клик на изображение, клик на название товара, клик на кнопку “купить” или “подробнее”), обратить внимание на то что есть диапазон, в котором в зависимости от количества меняется стоимость товара</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2 в поле “количество” ввести 1000, цена изменится до 40.46 за штуку
+3 в поле “количество” ввести 1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена возвращается к стартовому значению в 47.60 за единицу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена остается минимальной, так как это большая закупка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOB_22</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> на странице магазина перейти на карточку товара “Перекус для собачки” </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri (Body)"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">любым способом (клик на изображение, клик на название товара, клик на кнопку “купить” или “подробнее”), обратить внимание на то что есть диапазон, в котором в зависимости от количества меняется стоимость товара, цвет по умолчанию blue</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Выбрать цвет (color) blue или red 
+3 в поле “количество” ввести 100
+4 в поле “количество” ввести 1000
+5 в поле “количество” ввести 10001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 При вводе в поле “количество” числа 100, цена меняется до 110.07 за штуку для blue, или 114.57 за штуку для red
+2 При вводе в поле “количество” числа 1000, цена меняется до 103.96 за штуку для blue, или 108.21 за штуку для red
+3 При вводе в поле “количество” числа 10001, цена меняется до 122.30 за штуку для blue, или 127.30 за штуку для red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 При вводе в поле “количество” числа 100, цена меняется до 116.19 за штуку для blue, или 120.94 за штуку для red, так как это граница предыдущего диапазона (11-100)
+2 При вводе в поле “количество” числа 1000, цена меняется до 110.07 за штуку для blue, или 114.57 за штуку для red, так как это граница предыдущего диапазона (101-1000)
+3 При вводе в поле “количество” числа 10001, цена остается минимальной: 103.96 за штуку для blue, или 108.21 за штуку для red, так как крупный опт (выше 10000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOB_23</t>
   </si>
   <si>
     <t xml:space="preserve">Проверка </t>
@@ -871,10 +1013,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ304"/>
+  <dimension ref="A1:AMJ388"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A235" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B245" activeCellId="0" sqref="B245"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A316" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B309" activeCellId="0" sqref="B309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2216,13 +2358,17 @@
       <c r="A182" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B182" s="9"/>
+      <c r="B182" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B183" s="7"/>
+      <c r="B183" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3" t="s">
@@ -2312,13 +2458,17 @@
       <c r="A196" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B196" s="9"/>
+      <c r="B196" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B197" s="7"/>
+      <c r="B197" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="3" t="s">
@@ -2408,13 +2558,17 @@
       <c r="A210" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B210" s="9"/>
+      <c r="B210" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B211" s="7"/>
+      <c r="B211" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="3" t="s">
@@ -2504,13 +2658,17 @@
       <c r="A224" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B224" s="9"/>
+      <c r="B224" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B225" s="7"/>
+      <c r="B225" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3" t="s">
@@ -2598,13 +2756,17 @@
       <c r="A238" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B238" s="9"/>
+      <c r="B238" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B239" s="7"/>
+      <c r="B239" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="3" t="s">
@@ -2692,13 +2854,17 @@
       <c r="A252" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B252" s="9"/>
+      <c r="B252" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="253" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B253" s="7"/>
+      <c r="B253" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="254" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="3" t="s">
@@ -2720,27 +2886,31 @@
       <c r="A256" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B256" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B256" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="14"/>
-      <c r="B257" s="16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B257" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B258" s="7"/>
+      <c r="B258" s="7" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B259" s="17"/>
+      <c r="B259" s="17" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="260" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="3" t="s">
@@ -2769,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,20 +2947,24 @@
         <v>3</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B266" s="9"/>
+      <c r="B266" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B267" s="7"/>
+      <c r="B267" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="268" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="3" t="s">
@@ -2808,31 +2982,35 @@
         <v>107</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B270" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B270" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="14"/>
-      <c r="B271" s="16" t="n">
-        <v>2</v>
+      <c r="B271" s="16" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B272" s="7"/>
+      <c r="B272" s="7" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="273" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B273" s="17"/>
+      <c r="B273" s="17" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="3" t="s">
@@ -2861,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,20 +3047,24 @@
         <v>3</v>
       </c>
       <c r="B279" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B280" s="9"/>
+      <c r="B280" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B281" s="7"/>
+      <c r="B281" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="3" t="s">
@@ -2904,27 +3086,31 @@
       <c r="A284" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B284" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B284" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="14"/>
-      <c r="B285" s="16" t="n">
-        <v>2</v>
+      <c r="B285" s="16" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B286" s="7"/>
+      <c r="B286" s="7" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B287" s="17"/>
+      <c r="B287" s="17" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="3" t="s">
@@ -2953,7 +3139,7 @@
         <v>1</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,20 +3147,24 @@
         <v>3</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B294" s="9"/>
+      <c r="B294" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B295" s="7"/>
+      <c r="B295" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="3" t="s">
@@ -2992,31 +3182,35 @@
         <v>107</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B298" s="15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="299" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="14"/>
-      <c r="B299" s="16" t="n">
-        <v>2</v>
+      <c r="B299" s="16" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B300" s="7"/>
+      <c r="B300" s="7" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="301" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B301" s="17"/>
+      <c r="B301" s="17" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="3" t="s">
@@ -3040,8 +3234,568 @@
         <v>23</v>
       </c>
     </row>
+    <row r="306" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B306" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B307" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B308" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B309" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B310" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B311" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A312" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B312" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="14"/>
+      <c r="B313" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B314" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B315" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B316" s="18"/>
+    </row>
+    <row r="317" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B317" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B318" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A320" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B320" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B321" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A322" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B322" s="9"/>
+    </row>
+    <row r="323" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B323" s="7"/>
+    </row>
+    <row r="324" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B324" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B325" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A326" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B326" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="14"/>
+      <c r="B327" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B328" s="7"/>
+    </row>
+    <row r="329" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B329" s="17"/>
+    </row>
+    <row r="330" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A330" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B330" s="18"/>
+    </row>
+    <row r="331" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B331" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B332" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A335" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B335" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B336" s="9"/>
+    </row>
+    <row r="337" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B337" s="7"/>
+    </row>
+    <row r="338" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B338" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B339" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A340" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B340" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="14"/>
+      <c r="B341" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B342" s="7"/>
+    </row>
+    <row r="343" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B343" s="17"/>
+    </row>
+    <row r="344" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B344" s="18"/>
+    </row>
+    <row r="345" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B345" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B346" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B348" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A349" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B349" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B350" s="9"/>
+    </row>
+    <row r="351" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B351" s="7"/>
+    </row>
+    <row r="352" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B352" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B353" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A354" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B354" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="14"/>
+      <c r="B355" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B356" s="7"/>
+    </row>
+    <row r="357" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B357" s="17"/>
+    </row>
+    <row r="358" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B358" s="18"/>
+    </row>
+    <row r="359" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B359" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B360" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B362" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B363" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B364" s="9"/>
+    </row>
+    <row r="365" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A365" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B365" s="7"/>
+    </row>
+    <row r="366" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A366" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B366" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A367" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B367" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A368" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B368" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A369" s="14"/>
+      <c r="B369" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A370" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B370" s="7"/>
+    </row>
+    <row r="371" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A371" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B371" s="17"/>
+    </row>
+    <row r="372" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B372" s="18"/>
+    </row>
+    <row r="373" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B373" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B374" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B376" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A377" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B377" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A378" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B378" s="9"/>
+    </row>
+    <row r="379" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B379" s="7"/>
+    </row>
+    <row r="380" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B380" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B381" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A382" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B382" s="15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="14"/>
+      <c r="B383" s="16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B384" s="7"/>
+    </row>
+    <row r="385" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A385" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B385" s="17"/>
+    </row>
+    <row r="386" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A386" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B386" s="18"/>
+    </row>
+    <row r="387" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B387" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B388" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="28">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A23:A25"/>
@@ -3064,13 +3818,19 @@
     <mergeCell ref="A270:A271"/>
     <mergeCell ref="A284:A285"/>
     <mergeCell ref="A298:A299"/>
+    <mergeCell ref="A312:A313"/>
+    <mergeCell ref="A326:A327"/>
+    <mergeCell ref="A340:A341"/>
+    <mergeCell ref="A354:A355"/>
+    <mergeCell ref="A368:A369"/>
+    <mergeCell ref="A382:A383"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B19 B34 B49 B64 B79 B94 B109 B124 B139 B154 B168 B182 B196 B210 B224 B238 B252 B266 B280 B294" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5 B19 B34 B49 B64 B79 B94 B109 B124 B139 B154 B168 B182 B196 B210 B224 B238 B252 B266 B280 B294 B308 B322 B336 B350 B364 B378" type="list">
       <formula1>Sheet1!$H$94:$H$98</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6 B20 B35 B50 B65 B80 B95 B110 B125 B140 B155 B169 B183 B197 B211 B225 B239 B253 B267 B281 B295" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6 B20 B35 B50 B65 B80 B95 B110 B125 B140 B155 B169 B183 B197 B211 B225 B239 B253 B267 B281 B295 B309 B323 B337 B351 B365 B379" type="list">
       <formula1>Sheet1!$E$94:$E$96</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3104,6 +3864,12 @@
     <hyperlink ref="B269" r:id="rId26" display="https://qahacking.guru/index.php/magazin"/>
     <hyperlink ref="B283" r:id="rId27" display="https://qahacking.guru/index.php/magazin"/>
     <hyperlink ref="B297" r:id="rId28" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B311" r:id="rId29" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B325" r:id="rId30" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B339" r:id="rId31" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B353" r:id="rId32" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B367" r:id="rId33" display="https://qahacking.guru/index.php/magazin"/>
+    <hyperlink ref="B381" r:id="rId34" display="https://qahacking.guru/index.php/magazin"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>